<commit_message>
Finished Report Data/Outline. Troubleshooting pdf export.
</commit_message>
<xml_diff>
--- a/data/CFT Time Series (Clean).xlsx
+++ b/data/CFT Time Series (Clean).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissa/Library/CloudStorage/Dropbox/GitHub/PCCFA_25_28_negotiations/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365709E2-152B-C245-AB62-569F27493965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308B781E-0D00-2E49-80D4-31AB71B4E9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="16620" activeTab="6" xr2:uid="{15C1D82A-529D-984E-BC61-80A8779F00F2}"/>
   </bookViews>
@@ -5717,8 +5717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5855731F-37F9-D247-96A7-EEF3B9502E78}">
   <dimension ref="A1:Q74"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A28" sqref="A1:A1048576"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9621,8 +9621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8700D12-3028-3C4D-8270-7DD37C9FF1B9}">
   <dimension ref="A1:Q74"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A42" sqref="A1:A1048576"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17432,8 +17432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12279E9-7607-794D-9280-6816CD25706B}">
   <dimension ref="A1:Q73"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>